<commit_message>
Update MSME definitions and data files
</commit_message>
<xml_diff>
--- a/assets/data/MSME Country Indicators - Argentina Summary.xlsx
+++ b/assets/data/MSME Country Indicators - Argentina Summary.xlsx
@@ -103,40 +103,63 @@
     <t>Turnover (local currency, unless noted otherwise)</t>
   </si>
   <si>
-    <t>&lt;5 Indstr. &amp; trade&lt;br/&gt;&lt;4 Services</t>
+    <t>&lt;5 Indstr. &amp; trade
+&lt;4 Services</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>&lt;610,000 Agriculture, &lt;br/&gt;&lt;1,800,000 Industry, &lt;br/&gt;&lt;2,400,000 Trade, &lt;br/&gt;&lt;590,000 Services, &lt;br/&gt;&lt;760,000 Construction</t>
+    <t>&lt;610,000 Agriculture, 
+&lt;1,800,000 Industry, 
+&lt;2,400,000 Trade, 
+&lt;590,000 Services, 
+&lt;760,000 Construction</t>
   </si>
   <si>
     <t>Small</t>
   </si>
   <si>
-    <t>&lt;24 Indstr. &lt;br/&gt;&lt;23 Trade&lt;br/&gt;&lt;17 Services</t>
-  </si>
-  <si>
-    <t>&lt;4,100,000 Agriculture, &lt;br/&gt;&lt;10,300,000 Industry, &lt;br/&gt;&lt;14,000,000 Trade, &lt;br/&gt;&lt;4,300,000 Services, &lt;br/&gt;&lt;4,800,000 Construction</t>
+    <t>&lt;24 Indstr. 
+&lt;23 Trade
+&lt;17 Services</t>
+  </si>
+  <si>
+    <t>&lt;4,100,000 Agriculture, 
+&lt;10,300,000 Industry, 
+&lt;14,000,000 Trade, 
+&lt;4,300,000 Services, 
+&lt;4,800,000 Construction</t>
   </si>
   <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>&lt;96 Indstr. &lt;br/&gt;&lt;67 Trade&lt;br/&gt;&lt;66 Services</t>
-  </si>
-  <si>
-    <t>&lt;24,100,000 Agriculture, &lt;br/&gt;&lt;82,200,000 Industry, &lt;br/&gt;&lt;111,900,000 Trade, &lt;br/&gt;&lt;28,300,000 Services, &lt;br/&gt;&lt;37,700,000 Construction</t>
+    <t>&lt;96 Indstr. 
+&lt;67 Trade
+&lt;66 Services</t>
+  </si>
+  <si>
+    <t>&lt;24,100,000 Agriculture, 
+&lt;82,200,000 Industry, 
+&lt;111,900,000 Trade, 
+&lt;28,300,000 Services, 
+&lt;37,700,000 Construction</t>
   </si>
   <si>
     <t>Large</t>
   </si>
   <si>
-    <t>&gt;=96 Indstr.&lt;br/&gt; &gt;=67 Trade&lt;br/&gt;&gt;=66 Services</t>
-  </si>
-  <si>
-    <t>&gt;=24,100,000 Agriculture, &lt;br/&gt;&gt;=82,200,000 Industry, &lt;br/&gt;&gt;=111,900,000 Trade, &lt;br/&gt;&gt;=28,300,000 Services, &lt;br/&gt;&gt;=37,700,000 Construction</t>
+    <t>&gt;=96 Indstr.
+ &gt;=67 Trade
+&gt;=66 Services</t>
+  </si>
+  <si>
+    <t>&gt;=24,100,000 Agriculture, 
+&gt;=82,200,000 Industry, 
+&gt;=111,900,000 Trade, 
+&gt;=28,300,000 Services, 
+&gt;=37,700,000 Construction</t>
   </si>
   <si>
     <t>Sector Distribution Details</t>

</xml_diff>